<commit_message>
line 24 range updated
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Giga-bite pro\Vasudha\certigen\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B4EA2A-D130-4129-B473-FC7F2BCECAA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Name of Participant</t>
   </si>
@@ -39,7 +48,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -51,12 +60,9 @@
     <t>Laxya Pahuja</t>
   </si>
   <si>
-    <t>hackathon</t>
-  </si>
-  <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -68,15 +74,9 @@
     <t>Khwaish Gupta</t>
   </si>
   <si>
-    <t>life</t>
-  </si>
-  <si>
-    <t>Participation</t>
-  </si>
-  <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -84,38 +84,31 @@
       <t>khwaish.g@gmail.com</t>
     </r>
   </si>
+  <si>
+    <t>Debate</t>
+  </si>
+  <si>
+    <t>Hackathon</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color indexed="10"/>
       <name val="Calibri"/>
@@ -220,41 +213,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -263,25 +234,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -407,7 +438,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -416,7 +447,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -425,7 +456,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -499,7 +530,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -507,7 +538,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -526,7 +557,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -556,7 +587,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -582,7 +613,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -608,7 +639,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -634,7 +665,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -660,7 +691,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -686,7 +717,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -712,7 +743,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -738,7 +769,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -764,7 +795,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -777,9 +808,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -794,7 +831,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -802,7 +839,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -821,7 +858,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -847,7 +884,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -873,7 +910,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -899,7 +936,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -925,7 +962,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -951,7 +988,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -977,7 +1014,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1003,7 +1040,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1029,7 +1066,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1055,7 +1092,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1068,9 +1105,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1084,7 +1127,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1103,7 +1146,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1133,7 +1176,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1159,7 +1202,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1185,7 +1228,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1211,7 +1254,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1237,7 +1280,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1263,7 +1306,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1289,7 +1332,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1315,7 +1358,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1341,7 +1384,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1354,150 +1397,160 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1719" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="3">
+    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="3">
-        <v>10</v>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="3">
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s" s="5">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s" s="7">
-        <v>15</v>
-      </c>
+    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="7"/>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
+    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" location="" tooltip="" display="shizuka@ais.amity.edu"/>
-    <hyperlink ref="E3" r:id="rId2" location="" tooltip="" display="connieraff@yahoo.com"/>
-    <hyperlink ref="E4" r:id="rId3" location="" tooltip="" display="khwaish.g@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>